<commit_message>
criado bot para extrair do excel e preencher a folha de ponto do esocial
</commit_message>
<xml_diff>
--- a/batidas_HENRIQUE ARAUJO.xlsx
+++ b/batidas_HENRIQUE ARAUJO.xlsx
@@ -488,27 +488,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>08:00:16</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11:58</t>
+          <t>11:58:43</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12:58</t>
+          <t>12:58:08</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17:27</t>
+          <t>17:27:49</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>08:27:00</t>
+          <t>08:28:08</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -530,27 +530,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>07:54</t>
+          <t>07:54:02</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>12:18</t>
+          <t>12:18:26</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>13:21</t>
+          <t>13:21:26</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:31:39</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>08:34:00</t>
+          <t>08:34:37</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -572,27 +572,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>07:38:42</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10:59</t>
+          <t>10:59:53</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>11:56</t>
+          <t>11:56:57</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:13:22</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>08:38:00</t>
+          <t>08:37:36</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -614,27 +614,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>07:45</t>
+          <t>07:45:11</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10:48</t>
+          <t>10:48:22</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>11:45</t>
+          <t>11:45:46</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:14:53</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>08:32:00</t>
+          <t>08:32:18</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -656,27 +656,27 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>08:20</t>
+          <t>08:20:04</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>11:55</t>
+          <t>11:55:11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12:54</t>
+          <t>12:54:49</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:09:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>07:50:00</t>
+          <t>07:49:18</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -698,27 +698,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>07:44</t>
+          <t>07:44:18</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>11:57</t>
+          <t>11:57:22</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12:59</t>
+          <t>12:59:15</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:10:39</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>08:24:00</t>
+          <t>08:24:28</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -740,27 +740,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>07:53</t>
+          <t>07:53:53</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>11:28</t>
+          <t>11:28:55</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12:28</t>
+          <t>12:28:44</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:14:01</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>08:21:00</t>
+          <t>08:20:19</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -782,27 +782,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>08:03</t>
+          <t>08:03:17</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>11:35</t>
+          <t>11:35:20</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12:38</t>
+          <t>12:38:36</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:05:03</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>07:59:00</t>
+          <t>07:58:30</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -824,27 +824,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>08:09</t>
+          <t>08:09:52</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11:13</t>
+          <t>11:13:59</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12:15</t>
+          <t>12:15:31</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:06:03</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>07:55:00</t>
+          <t>07:54:39</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -866,27 +866,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>07:45</t>
+          <t>07:45:19</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11:51</t>
+          <t>11:51:59</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>12:55:19</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>17:05</t>
+          <t>17:05:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>08:16:00</t>
+          <t>08:16:21</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -908,27 +908,27 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>07:47:59</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:06:28</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12:56</t>
+          <t>12:56:45</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17:17</t>
+          <t>17:17:02</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>08:40:00</t>
+          <t>08:38:46</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -950,27 +950,27 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>07:42</t>
+          <t>07:42:01</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11:14</t>
+          <t>11:14:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12:13</t>
+          <t>12:13:59</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>17:30:04</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>08:49:00</t>
+          <t>08:48:38</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -992,27 +992,27 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>07:59</t>
+          <t>07:59:57</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11:48</t>
+          <t>11:48:40</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12:48</t>
+          <t>12:48:40</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>17:32</t>
+          <t>17:32:47</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>08:33:00</t>
+          <t>08:32:50</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1034,32 +1034,32 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>07:33</t>
+          <t>07:33:39</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11:59</t>
+          <t>11:59:56</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12:57</t>
+          <t>12:57:46</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:33:40</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>09:02:00</t>
+          <t>09:02:11</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>00:12:00</t>
+          <t>00:12:11</t>
         </is>
       </c>
     </row>
@@ -1076,32 +1076,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>07:38</t>
+          <t>07:38:33</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11:27</t>
+          <t>11:27:13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12:26</t>
+          <t>12:26:27</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:31:35</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>08:54:00</t>
+          <t>08:53:48</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>00:04:00</t>
+          <t>00:03:48</t>
         </is>
       </c>
     </row>
@@ -1118,32 +1118,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>07:42</t>
+          <t>07:42:53</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>11:39</t>
+          <t>11:39:24</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12:37</t>
+          <t>12:37:24</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>17:31</t>
+          <t>17:31:52</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>08:51:00</t>
+          <t>08:50:59</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>00:01:00</t>
+          <t>00:00:59</t>
         </is>
       </c>
     </row>
@@ -1160,27 +1160,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>08:06</t>
+          <t>08:06:11</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12:06</t>
+          <t>12:06:11</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>13:06</t>
+          <t>13:06:11</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>17:42:42</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>08:36:00</t>
+          <t>08:36:31</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1202,12 +1202,12 @@
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
-          <t>144:21:00</t>
+          <t>144:19:57</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>00:17:00</t>
+          <t>00:16:58</t>
         </is>
       </c>
     </row>

</xml_diff>